<commit_message>
FedRAMP Selection Controls Worksheet
</commit_message>
<xml_diff>
--- a/assets/resources/templates/FedRAMP-Selection-Controls-Worksheet.xlsx
+++ b/assets/resources/templates/FedRAMP-Selection-Controls-Worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shiva.alipour/Library/CloudStorage/GoogleDrive-shiva.alipour@theclearing.com/.shortcut-targets-by-id/0B-kDjNiRnhdvTS13YjR2d0VyTGM/Graphics/TC Visual Design/Client/GSA/FedRAMP/Documents/GSA-4783 FedRAMP Rev5 Updates/In Progress/Selection Controls Worksheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80CC743A-96A1-9A43-BBED-BA74C84F51ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76705AC0-32A3-8B40-AB6B-AE73D3B9AE17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="760" windowWidth="25160" windowHeight="20000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1821,11 +1821,23 @@
     <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="14" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1839,15 +1851,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1858,9 +1861,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="14" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2197,103 +2197,103 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="2" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="58" t="s">
         <v>407</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
     </row>
     <row r="2" spans="1:10" s="5" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="59" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
     </row>
     <row r="3" spans="1:10" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.15">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
       <c r="J3" s="11"/>
     </row>
     <row r="4" spans="1:10" s="14" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="55" t="s">
         <v>382</v>
       </c>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
       <c r="J4" s="13"/>
     </row>
     <row r="5" spans="1:10" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="54" t="s">
+      <c r="A5" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
-      <c r="H5" s="55"/>
-      <c r="I5" s="55"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="56"/>
+      <c r="H5" s="56"/>
+      <c r="I5" s="56"/>
       <c r="J5" s="13"/>
     </row>
     <row r="6" spans="1:10" s="14" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="55" t="s">
         <v>383</v>
       </c>
-      <c r="B6" s="54"/>
-      <c r="C6" s="54"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="55"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="56"/>
       <c r="J6" s="13"/>
     </row>
     <row r="7" spans="1:10" s="5" customFormat="1" ht="65.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="56" t="s">
+      <c r="A7" s="60" t="s">
         <v>96</v>
       </c>
-      <c r="B7" s="56"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="56" t="s">
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="60" t="s">
         <v>164</v>
       </c>
-      <c r="G7" s="58"/>
-      <c r="H7" s="58"/>
-      <c r="I7" s="59"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="63"/>
       <c r="J7" s="7" t="s">
         <v>95</v>
       </c>
@@ -5100,18 +5100,18 @@
     <sortCondition ref="B9:B146"/>
   </sortState>
   <mergeCells count="12">
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="F7:I7"/>
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="F4:I4"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="F3:I3"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="F7:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5141,103 +5141,103 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="2" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="58" t="s">
         <v>408</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="59" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
     </row>
     <row r="3" spans="1:10" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.15">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
       <c r="J3" s="11"/>
     </row>
     <row r="4" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="55" t="s">
         <v>382</v>
       </c>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
       <c r="J4" s="13"/>
     </row>
     <row r="5" spans="1:10" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="54" t="s">
+      <c r="A5" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
-      <c r="H5" s="55"/>
-      <c r="I5" s="55"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="56"/>
+      <c r="H5" s="56"/>
+      <c r="I5" s="56"/>
       <c r="J5" s="13"/>
     </row>
     <row r="6" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="55" t="s">
         <v>383</v>
       </c>
-      <c r="B6" s="54"/>
-      <c r="C6" s="54"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="55"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="56"/>
       <c r="J6" s="13"/>
     </row>
     <row r="7" spans="1:10" s="2" customFormat="1" ht="65.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="56" t="s">
+      <c r="A7" s="60" t="s">
         <v>96</v>
       </c>
-      <c r="B7" s="56"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="63" t="s">
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="64" t="s">
         <v>164</v>
       </c>
-      <c r="G7" s="58"/>
-      <c r="H7" s="58"/>
-      <c r="I7" s="59"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="63"/>
       <c r="J7" s="7" t="s">
         <v>95</v>
       </c>
@@ -8005,18 +8005,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="F7:I7"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="F3:I3"/>
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="F4:I4"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="F7:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8046,103 +8046,103 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="12" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="58" t="s">
         <v>409</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
     </row>
     <row r="2" spans="1:10" s="12" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="59" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
     </row>
     <row r="3" spans="1:10" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.15">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
       <c r="J3" s="26"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="55" t="s">
         <v>382</v>
       </c>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
       <c r="J4" s="3"/>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="54" t="s">
+      <c r="A5" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
-      <c r="H5" s="55"/>
-      <c r="I5" s="55"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="56"/>
+      <c r="H5" s="56"/>
+      <c r="I5" s="56"/>
       <c r="J5" s="3"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="55" t="s">
         <v>383</v>
       </c>
-      <c r="B6" s="54"/>
-      <c r="C6" s="54"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="55"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="56"/>
       <c r="J6" s="3"/>
     </row>
     <row r="7" spans="1:10" s="12" customFormat="1" ht="65.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="56" t="s">
+      <c r="A7" s="60" t="s">
         <v>96</v>
       </c>
-      <c r="B7" s="56"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="63" t="s">
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="64" t="s">
         <v>164</v>
       </c>
-      <c r="G7" s="58"/>
-      <c r="H7" s="58"/>
-      <c r="I7" s="59"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="63"/>
       <c r="J7" s="7" t="s">
         <v>95</v>
       </c>
@@ -10557,18 +10557,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="F7:I7"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="F3:I3"/>
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="F4:I4"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="F7:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10599,22 +10599,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="49" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="58" t="s">
         <v>410</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
     </row>
     <row r="2" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="65" t="s">
         <v>399</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
     </row>
     <row r="3" spans="1:5" ht="75" x14ac:dyDescent="0.15">
       <c r="A3" s="34" t="s">
@@ -12124,22 +12124,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="58" t="s">
         <v>411</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
     </row>
     <row r="2" spans="1:5" ht="37" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="65" t="s">
         <v>399</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
     </row>
     <row r="3" spans="1:5" ht="75" x14ac:dyDescent="0.15">
       <c r="A3" s="34" t="s">
@@ -13350,22 +13350,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="58" t="s">
         <v>412</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
     </row>
     <row r="2" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="65" t="s">
         <v>399</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
     </row>
     <row r="3" spans="1:5" ht="75" x14ac:dyDescent="0.15">
       <c r="A3" s="34" t="s">
@@ -13975,11 +13975,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="49" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="58" t="s">
         <v>413</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
     </row>
     <row r="2" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="35" t="s">
@@ -16081,14 +16081,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="49" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="58" t="s">
         <v>414</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="58"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="62"/>
     </row>
     <row r="2" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="35" t="s">
@@ -18728,12 +18728,12 @@
       <c r="D1" s="52"/>
     </row>
     <row r="2" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="65" t="s">
+      <c r="A2" s="66" t="s">
         <v>400</v>
       </c>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
     </row>
     <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A3" s="53" t="s">
@@ -18756,7 +18756,7 @@
       <c r="B4" s="46" t="s">
         <v>406</v>
       </c>
-      <c r="C4" s="67">
+      <c r="C4" s="54">
         <v>1</v>
       </c>
       <c r="D4" s="47" t="s">

</xml_diff>